<commit_message>
Add fired as the number of executed rules
</commit_message>
<xml_diff>
--- a/src/test/resources/character-unit-test.xlsx
+++ b/src/test/resources/character-unit-test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Test Name</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>fired</t>
   </si>
 </sst>
 </file>
@@ -230,13 +239,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -638,10 +648,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -650,7 +660,7 @@
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,8 +685,11 @@
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1">
+    <row r="2" spans="1:9" s="2" customFormat="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -698,8 +711,11 @@
       <c r="G2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" s="4" customFormat="1">
+    <row r="3" spans="1:9" s="4" customFormat="1">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -721,8 +737,11 @@
       <c r="G3" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" s="2" customFormat="1">
+    <row r="4" spans="1:9" s="2" customFormat="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -744,8 +763,11 @@
       <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" s="2" customFormat="1">
+    <row r="5" spans="1:9" s="2" customFormat="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -767,8 +789,11 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="I5" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" s="4" customFormat="1">
+    <row r="6" spans="1:9" s="4" customFormat="1">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -790,8 +815,11 @@
       <c r="G6" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1">
+    <row r="7" spans="1:9" s="2" customFormat="1">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -815,6 +843,36 @@
       </c>
       <c r="H7" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>